<commit_message>
[ADDED] - Blog Carousel
</commit_message>
<xml_diff>
--- a/data/blog_layout.xlsx
+++ b/data/blog_layout.xlsx
@@ -5,13 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1_2_2_2" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Hoja1_2" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Hoja1_2_2" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Hoja1" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Hoja1_3" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="Hoja1_3_2" sheetId="6" state="visible" r:id="rId8"/>
+    <sheet name="Hoja1_3_2_2" sheetId="7" state="visible" r:id="rId9"/>
+    <sheet name="Hoja1_3_2_2_2" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="Hoja1_3_2_2_2_2" sheetId="9" state="visible" r:id="rId11"/>
+    <sheet name="Hoja1_3_2_2_2_2_2" sheetId="10" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="93">
   <si>
     <t xml:space="preserve">Numero</t>
   </si>
@@ -288,6 +294,24 @@
   <si>
     <t xml:space="preserve">2023 está destinado a ser un año de reducción del consumismo, con más énfasis en la reparación, el reciclaje, la reutilización y el ahorro. Los minoristas ya comenzaron a adaptarse a este cambio, con empresas como REI, lululemon, Levi, Walmart, Patagonia, Everlane y Eileen Fisher, todas ofreciendo productos usados o una mayor transparencia en las cadenas de suministro. A medida que la Generación Z crece en influencia y gana más dinero, es probable que las empresas que dan prioridad a la sostenibilidad sean las ganadoras finales.
 Estas cinco de las tendencias minoristas mencionadas anteriormente son las más relevantes para la industria. Además, los minoristas deben considerar la remodelación de la fuerza laboral, como encontrar el equilibrio adecuado entre el trabajo en el sitio y remoto, así como la creación de una atmósfera de inclusión. Además, la comunidad debe ser una parte integral de la estrategia de inversión. A medida que el año se acerca a su fin, los minoristas deben permanecer enfocados en el viaje del comprador para un futuro exitoso.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post de Ejemplo No.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post de Ejemplo No.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post de Ejemplo No.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post de Ejemplo No.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post de Ejemplo No.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post de Ejemplo No.10</t>
   </si>
 </sst>
 </file>
@@ -569,8 +593,8 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -896,6 +920,455 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I50"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="52.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="9.34"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>2023</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="58.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="147.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="390.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="369.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="327.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="312.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="485.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="8"/>
+    </row>
+    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="8"/>
+    </row>
+    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="8"/>
+    </row>
+    <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="8"/>
+    </row>
+    <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+    </row>
+    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1"/>
@@ -2079,4 +2552,2249 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I50"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="52.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="9.34"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>2023</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="58.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="147.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="390.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="369.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="327.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="312.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="485.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="8"/>
+    </row>
+    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="8"/>
+    </row>
+    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="8"/>
+    </row>
+    <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="8"/>
+    </row>
+    <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+    </row>
+    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I50"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="52.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="9.34"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>2023</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="58.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="147.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="390.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="369.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="327.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="312.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="485.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="8"/>
+    </row>
+    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="8"/>
+    </row>
+    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="8"/>
+    </row>
+    <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="8"/>
+    </row>
+    <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+    </row>
+    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I50"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="52.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="9.34"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>2023</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="58.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="147.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="390.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="369.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="327.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="312.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="485.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="8"/>
+    </row>
+    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="8"/>
+    </row>
+    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="8"/>
+    </row>
+    <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="8"/>
+    </row>
+    <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+    </row>
+    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I50"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="52.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="9.34"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>2023</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="58.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="147.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="390.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="369.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="327.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="312.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="485.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="8"/>
+    </row>
+    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="8"/>
+    </row>
+    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="8"/>
+    </row>
+    <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="8"/>
+    </row>
+    <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+    </row>
+    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I50"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="52.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="9.34"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>2023</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="58.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="147.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="390.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="369.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="327.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="312.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="485.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="8"/>
+    </row>
+    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="8"/>
+    </row>
+    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="8"/>
+    </row>
+    <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="8"/>
+    </row>
+    <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+    </row>
+    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added - gallery functions
</commit_message>
<xml_diff>
--- a/data/blog_layout.xlsx
+++ b/data/blog_layout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1_2_2_2" sheetId="1" state="visible" r:id="rId3"/>
@@ -593,7 +593,7 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -942,7 +942,7 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -951,7 +951,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="52.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="9.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="9.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1391,7 +1391,7 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -1750,7 +1750,7 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2112,7 +2112,7 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2561,7 +2561,7 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -2570,7 +2570,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="52.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="9.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="9.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3010,7 +3010,7 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -3019,7 +3019,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="52.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="9.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="9.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3459,7 +3459,7 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -3468,7 +3468,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="52.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="9.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="9.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3908,7 +3908,7 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3917,7 +3917,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="52.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="9.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="9.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4357,7 +4357,7 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4366,7 +4366,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="52.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="9.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="9.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>